<commit_message>
Working on file structure
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27B162CE-8D5F-4EF5-B0E9-EDADAFB7B122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DC513E-CC5D-49DC-B12B-27E7976FDA3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
+    <workbookView xWindow="14295" yWindow="360" windowWidth="14610" windowHeight="15240" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -141,10 +147,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -463,7 +470,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,12 +563,15 @@
         <v>3</v>
       </c>
       <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -569,12 +579,14 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -582,6 +594,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Planning, agenda, basic presentation
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DC513E-CC5D-49DC-B12B-27E7976FDA3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63815581-C581-4298-92A7-24C2A9388514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="360" windowWidth="14610" windowHeight="15240" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
+    <workbookView xWindow="28680" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Description</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Function parser</t>
   </si>
   <si>
-    <t>Physics</t>
-  </si>
-  <si>
     <t>Course input-output module</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Menu UI / course designer</t>
   </si>
   <si>
-    <t>Make it a game</t>
-  </si>
-  <si>
     <t>Aaron</t>
   </si>
   <si>
@@ -93,6 +87,27 @@
   </si>
   <si>
     <t>Function parser + physics</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Make it a game / merge / bug fixing</t>
+  </si>
+  <si>
+    <t>Game rules (scoring, keeping track of shots and hitting the water)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physics </t>
+  </si>
+  <si>
+    <t>In-game UI for shooting</t>
+  </si>
+  <si>
+    <t>Handle being out of bounds</t>
+  </si>
+  <si>
+    <t>UI and terrain improvements (if time allows)</t>
   </si>
 </sst>
 </file>
@@ -467,44 +482,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="56.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -512,16 +527,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -546,13 +561,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -567,7 +582,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
@@ -575,7 +590,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -583,14 +598,14 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -598,17 +613,35 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Planning phase 2 (and part of phase 3)
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255A1B72-80C4-4070-B040-A56339B65114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DA0981-1C93-4C35-8002-E6E7506E2A07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,32 +33,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Game rules</t>
-  </si>
-  <si>
-    <t>In-game UI</t>
-  </si>
-  <si>
-    <t>Function parser</t>
-  </si>
-  <si>
-    <t>Course input-output module</t>
-  </si>
-  <si>
-    <t>2 Game modes</t>
-  </si>
-  <si>
     <t>René</t>
   </si>
   <si>
-    <t>Menu UI / course designer</t>
-  </si>
-  <si>
     <t>Aaron</t>
   </si>
   <si>
@@ -75,47 +56,125 @@
     <t>Huan</t>
   </si>
   <si>
-    <t>3D model for ball and pole (in-engine)</t>
-  </si>
-  <si>
-    <t>3D models for ball and pole  (in-engine)</t>
-  </si>
-  <si>
-    <t>Menu UI / Course desginer</t>
-  </si>
-  <si>
-    <t>2 Game modes + Course input-output module + help on physics</t>
-  </si>
-  <si>
-    <t>Function parser + physics</t>
-  </si>
-  <si>
-    <t>Presentation</t>
-  </si>
-  <si>
-    <t>Make it a game / merge / bug fixing</t>
-  </si>
-  <si>
-    <t>Game rules (scoring, keeping track of shots and hitting the water)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Physics </t>
-  </si>
-  <si>
-    <t>In-game UI for shooting</t>
-  </si>
-  <si>
-    <t>Handle being out of bounds</t>
-  </si>
-  <si>
-    <t>UI and terrain improvements (if time allows)</t>
+    <t>Project structure</t>
+  </si>
+  <si>
+    <t>Connection UI and backend</t>
+  </si>
+  <si>
+    <t>Redo UI</t>
+  </si>
+  <si>
+    <t>Second order Verlet solver</t>
+  </si>
+  <si>
+    <t>Classical 4th order Runge Kutta solver</t>
+  </si>
+  <si>
+    <t>3D UI improvements (ball reset preview, shot direction indicator)</t>
+  </si>
+  <si>
+    <t>Music/sound effects</t>
+  </si>
+  <si>
+    <t>March 23-29</t>
+  </si>
+  <si>
+    <t>March 30 April 5</t>
+  </si>
+  <si>
+    <t>April 6-12</t>
+  </si>
+  <si>
+    <t>April 13-19</t>
+  </si>
+  <si>
+    <t>April 20-26</t>
+  </si>
+  <si>
+    <t>April 27 - May 3</t>
+  </si>
+  <si>
+    <t>May 4-10</t>
+  </si>
+  <si>
+    <t>May 11-17</t>
+  </si>
+  <si>
+    <t>May 18/19</t>
+  </si>
+  <si>
+    <t>Create new 3D engine</t>
+  </si>
+  <si>
+    <t>Create new 2D engine</t>
+  </si>
+  <si>
+    <t>in class</t>
+  </si>
+  <si>
+    <t>Multiplayer (turn based or switch after goal?)</t>
+  </si>
+  <si>
+    <t>Improved terrain and water</t>
+  </si>
+  <si>
+    <t>Basic bot research</t>
+  </si>
+  <si>
+    <t>Basic version of basic bot</t>
+  </si>
+  <si>
+    <t>Finished basic bot</t>
+  </si>
+  <si>
+    <t>Consider flying balls (phase 3 prep)</t>
+  </si>
+  <si>
+    <t>Research advanced bot (phase3)</t>
+  </si>
+  <si>
+    <t>Get started with advanced bot (phase3)</t>
+  </si>
+  <si>
+    <t>Bouncing against trees</t>
+  </si>
+  <si>
+    <t>Have a playable game (for humans)</t>
+  </si>
+  <si>
+    <t>Course designer basics (phase 3)</t>
+  </si>
+  <si>
+    <t>Course designer finished, including saving/loading (phase 3)</t>
+  </si>
+  <si>
+    <t>Support Ivan with the bot (research and implementation for basic and advanced bot)</t>
+  </si>
+  <si>
+    <t>Create 3D engine, create basis of 2D engine, improve project structure, expand 3D UI, 3D course designer, course desginer save/load system, improved terrain and water rendering</t>
+  </si>
+  <si>
+    <t>Music and sound effect, 'mutliplayer'</t>
+  </si>
+  <si>
+    <t>Second order Verlet solver, classic 4th order Runge Kutta solver, bouncing against trees, consider flying balls</t>
+  </si>
+  <si>
+    <t>Improve project structure, ensure that we have a playable game, bot research and development (basic and advanced)</t>
+  </si>
+  <si>
+    <t>Expand 2D engine, redo 2D UI,  connection UI and backend</t>
+  </si>
+  <si>
+    <t>Start with report (mainly structure)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +185,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -145,12 +212,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -158,18 +224,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Check Cell" xfId="2" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -483,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,160 +581,376 @@
     <col min="1" max="1" width="56.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1">
-        <v>43906</v>
-      </c>
-      <c r="C9" s="1">
-        <v>43907</v>
-      </c>
-      <c r="D9" s="1">
-        <v>43908</v>
-      </c>
-      <c r="E9" s="1">
-        <v>43909</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B7:Q7"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="B6:Q6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Schedule, who did what, agenda meeting
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DA0981-1C93-4C35-8002-E6E7506E2A07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849956D0-4848-4310-9DFE-6F9C46B02335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Matthijs</t>
   </si>
   <si>
-    <t>Huan</t>
-  </si>
-  <si>
     <t>Project structure</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>Start with report (mainly structure)</t>
+  </si>
+  <si>
+    <t>Haoran</t>
   </si>
 </sst>
 </file>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -609,7 +609,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -632,7 +632,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -655,7 +655,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -678,7 +678,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -698,10 +698,10 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -742,36 +742,36 @@
         <v>0</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="1"/>
@@ -785,7 +785,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -799,65 +799,65 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>7</v>
+      </c>
       <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -865,62 +865,62 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -928,14 +928,15 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -952,5 +953,8 @@
     <mergeCell ref="B6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D8:F8" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reformated planning and updated Who did what phase 1
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849956D0-4848-4310-9DFE-6F9C46B02335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2082FAF-2DC5-4CA5-95C4-B4756A041D88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
   <si>
     <t>Description</t>
   </si>
@@ -41,9 +41,6 @@
     <t>René</t>
   </si>
   <si>
-    <t>Aaron</t>
-  </si>
-  <si>
     <t>Ivan</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>in class</t>
   </si>
   <si>
-    <t>Multiplayer (turn based or switch after goal?)</t>
-  </si>
-  <si>
     <t>Improved terrain and water</t>
   </si>
   <si>
@@ -134,9 +128,6 @@
     <t>Get started with advanced bot (phase3)</t>
   </si>
   <si>
-    <t>Bouncing against trees</t>
-  </si>
-  <si>
     <t>Have a playable game (for humans)</t>
   </si>
   <si>
@@ -146,28 +137,97 @@
     <t>Course designer finished, including saving/loading (phase 3)</t>
   </si>
   <si>
-    <t>Support Ivan with the bot (research and implementation for basic and advanced bot)</t>
-  </si>
-  <si>
-    <t>Create 3D engine, create basis of 2D engine, improve project structure, expand 3D UI, 3D course designer, course desginer save/load system, improved terrain and water rendering</t>
-  </si>
-  <si>
-    <t>Music and sound effect, 'mutliplayer'</t>
-  </si>
-  <si>
-    <t>Second order Verlet solver, classic 4th order Runge Kutta solver, bouncing against trees, consider flying balls</t>
-  </si>
-  <si>
-    <t>Improve project structure, ensure that we have a playable game, bot research and development (basic and advanced)</t>
-  </si>
-  <si>
-    <t>Expand 2D engine, redo 2D UI,  connection UI and backend</t>
-  </si>
-  <si>
     <t>Start with report (mainly structure)</t>
   </si>
   <si>
     <t>Haoran</t>
+  </si>
+  <si>
+    <t>Who?</t>
+  </si>
+  <si>
+    <t>René and Jean</t>
+  </si>
+  <si>
+    <t>René and Ivan</t>
+  </si>
+  <si>
+    <t>René, Jean and Ivan</t>
+  </si>
+  <si>
+    <t>Bouncing against trees (phase 3)</t>
+  </si>
+  <si>
+    <t>Aaron and Ivan</t>
+  </si>
+  <si>
+    <t>Jean, Matthijs and René</t>
+  </si>
+  <si>
+    <t>Extended description</t>
+  </si>
+  <si>
+    <t>Create a new 3D engine using lwjgl</t>
+  </si>
+  <si>
+    <t>Add 2D options to the engine for UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make sure that the project structure is clear and flexible </t>
+  </si>
+  <si>
+    <t>Create an improved version of the phase 1 UI in the new engine</t>
+  </si>
+  <si>
+    <t>Make sure that the back- and frontend can properly communicate</t>
+  </si>
+  <si>
+    <t>Have a working game where you can at least shoot the ball and score</t>
+  </si>
+  <si>
+    <t>Implement the second order Verlet solver for physics</t>
+  </si>
+  <si>
+    <t>Implement the classical 4th order Runge kutta solver for physics</t>
+  </si>
+  <si>
+    <t>Add the physics for bouncing against trees, including hit detection</t>
+  </si>
+  <si>
+    <t>Figure out how a bot should work to meet the requirements for phase 2</t>
+  </si>
+  <si>
+    <t>Come up with an improved bot by doing research</t>
+  </si>
+  <si>
+    <t>Start the implementation of this improved bot</t>
+  </si>
+  <si>
+    <t>Enable the user to customize the terrain by adding sand and trees</t>
+  </si>
+  <si>
+    <t>Add a save and load option to the course designer</t>
+  </si>
+  <si>
+    <t>Improve the visuals for the terrain and water</t>
+  </si>
+  <si>
+    <t>Add 3D UI for resetting the ball and indicating in which direction you're shooting</t>
+  </si>
+  <si>
+    <t>Add music that plays while playing the game and add sound effects to actions like shooting and scoring</t>
+  </si>
+  <si>
+    <t>Create a first version of the bot for phase 2 that can already meet the requirements</t>
+  </si>
+  <si>
+    <t>Improve the bot further and fix any problems that the bot may have</t>
+  </si>
+  <si>
+    <t>Add the physics for flying balls and make sure the rest of the game still works when this is used</t>
+  </si>
+  <si>
+    <t>Prepare an outline for the report in LaTeX and learn LaTeX if needed</t>
   </si>
 </sst>
 </file>
@@ -245,7 +305,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -254,6 +314,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="2" builtinId="23" customBuiltin="1"/>
@@ -570,391 +636,450 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="15" max="15" width="73.7109375" customWidth="1"/>
+    <col min="17" max="17" width="57" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="M1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="M2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="M3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="M4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="M5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="M6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="M7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="M8" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="M9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="5"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="M10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="5"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="M11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="5"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="M12" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="5"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="M13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="5"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="M14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="M15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
       </c>
       <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M18" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M19" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M20" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
       <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="M21" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>43</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="M22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B7:Q7"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="B6:Q6"/>
+  <mergeCells count="21">
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="D8:F8" twoDigitTextYear="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sand painting works and it looks incredible! (Also updated the planning for Haoran)
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F214DF4-6911-4FDD-9A23-3B0366B4C33E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9744026D-A79A-4A31-B235-617A2BBCC61D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24990" yWindow="630" windowWidth="7500" windowHeight="6000" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
+    <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>Description</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>Prepare an outline for the report in LaTeX and learn LaTeX if needed</t>
+  </si>
+  <si>
+    <t>Additional engine improvements (shadows, improved AA)</t>
+  </si>
+  <si>
+    <t>Implement some additional and optional engine improvements</t>
   </si>
 </sst>
 </file>
@@ -318,7 +324,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -331,12 +337,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -654,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +686,7 @@
       <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -703,11 +711,11 @@
         <v>20</v>
       </c>
       <c r="L1" s="5"/>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
@@ -724,7 +732,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="12"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -732,11 +740,11 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="5"/>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
@@ -749,13 +757,13 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="13"/>
+      <c r="E4" s="12"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
@@ -768,13 +776,13 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="13"/>
+      <c r="F5" s="12"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
@@ -788,11 +796,11 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
@@ -806,11 +814,11 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
@@ -841,11 +849,11 @@
         <v>23</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="M9" s="8" t="s">
+      <c r="M9" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
       <c r="P9" s="5"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -858,11 +866,11 @@
       <c r="D10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="M10" s="8" t="s">
+      <c r="M10" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -873,11 +881,11 @@
         <v>41</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
       <c r="P11" s="5"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -890,11 +898,11 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
       <c r="P12" s="5"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -922,11 +930,11 @@
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="M14" s="8" t="s">
+      <c r="M14" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -937,11 +945,11 @@
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="M15" s="8" t="s">
+      <c r="M15" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -952,11 +960,11 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="M16" s="8" t="s">
+      <c r="M16" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -967,27 +975,28 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="M17" s="8" t="s">
+      <c r="M17" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="E18" s="9"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="13"/>
-      <c r="M18" s="8" t="s">
+      <c r="G18" s="2"/>
+      <c r="H18" s="9"/>
+      <c r="M18" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1000,11 +1009,11 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="M19" s="8" t="s">
+      <c r="M19" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1016,11 +1025,11 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="M20" s="8" t="s">
+      <c r="M20" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1032,63 +1041,92 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="M21" s="8" t="s">
+      <c r="M21" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-    </row>
-    <row r="22" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="M24" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+    </row>
+    <row r="22" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="M22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+    </row>
+    <row r="23" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+    </row>
+    <row r="24" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
     </row>
+    <row r="25" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="M27" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="M18:O18"/>
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="M7:O7"/>
     <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M26:O26"/>
     <mergeCell ref="M3:O3"/>
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="M5:O5"/>
@@ -1101,10 +1139,6 @@
     <mergeCell ref="M20:O20"/>
     <mergeCell ref="M21:O21"/>
     <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M18:O18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Improved planning, with headers
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9744026D-A79A-4A31-B235-617A2BBCC61D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A5FBB-EB04-4814-A454-AD73170E69A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
   <si>
     <t>Description</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Matthijs</t>
   </si>
   <si>
-    <t>Project structure</t>
-  </si>
-  <si>
     <t>Connection UI and backend</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>Create new 3D engine</t>
   </si>
   <si>
-    <t>Create new 2D engine</t>
-  </si>
-  <si>
     <t>in class</t>
   </si>
   <si>
@@ -146,18 +140,9 @@
     <t>Who?</t>
   </si>
   <si>
-    <t>René and Jean</t>
-  </si>
-  <si>
-    <t>René and Ivan</t>
-  </si>
-  <si>
     <t>René, Jean and Ivan</t>
   </si>
   <si>
-    <t>Bouncing against trees (phase 3)</t>
-  </si>
-  <si>
     <t>Aaron and Ivan</t>
   </si>
   <si>
@@ -170,12 +155,6 @@
     <t>Create a new 3D engine using lwjgl</t>
   </si>
   <si>
-    <t>Add 2D options to the engine for UI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make sure that the project structure is clear and flexible </t>
-  </si>
-  <si>
     <t>Create an improved version of the phase 1 UI in the new engine</t>
   </si>
   <si>
@@ -234,13 +213,67 @@
   </si>
   <si>
     <t>Implement some additional and optional engine improvements</t>
+  </si>
+  <si>
+    <t>Create new 2D engine basis</t>
+  </si>
+  <si>
+    <t>Expand 2D engine with buttons, textfields and a file explorer</t>
+  </si>
+  <si>
+    <t>Add the option to add 2D elements to the UI</t>
+  </si>
+  <si>
+    <t>PROJECT STRUCTURE AND PHASE 1 FIXES</t>
+  </si>
+  <si>
+    <t>GRAPHICS ENGINE</t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>BOT</t>
+  </si>
+  <si>
+    <t>REPORT</t>
+  </si>
+  <si>
+    <t>Bouncing against trees (phase 3 prep)</t>
+  </si>
+  <si>
+    <t>PRESENTATION</t>
+  </si>
+  <si>
+    <t>Create the presentation</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>Improve the graphics engine structure</t>
+  </si>
+  <si>
+    <t>Improve the physics engine structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">René </t>
+  </si>
+  <si>
+    <t>Make sure that the project structure is clear and flexible, focusing on the graphicsc engine's structure</t>
+  </si>
+  <si>
+    <t>Make sure that the project structure is clear and flexible, focusing on the physics engine's structure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,8 +303,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +338,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -318,13 +370,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -345,11 +398,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Check Cell" xfId="2" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -662,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,41 +742,41 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="L1" s="5"/>
-      <c r="M1" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
+      <c r="M1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
@@ -723,422 +784,505 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
+    <row r="3" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="12"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="L4" s="14"/>
+      <c r="M4" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+    </row>
+    <row r="5" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="12"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+    </row>
+    <row r="6" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="12"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="F6" s="12"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>35</v>
+      </c>
       <c r="E7" s="2"/>
+      <c r="F7" s="20"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
+      <c r="M7" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="M8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="12"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
       <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="M9" s="13" t="s">
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:17" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+    </row>
+    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+    </row>
+    <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="M13" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="M10" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="M11" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="5"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="M12" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="5"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="M13" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="5"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+    </row>
+    <row r="14" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
       <c r="M14" s="13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+    <row r="15" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2"/>
       <c r="M15" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="M16" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
+      <c r="E17" s="9"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="M17" s="13" t="s">
+      <c r="H17" s="9"/>
+      <c r="M17" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+    </row>
+    <row r="18" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="M18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+    </row>
+    <row r="20" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A20" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="20"/>
+      <c r="M21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="M22" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="5"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="M23" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="5"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="15"/>
+      <c r="M24" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K25" s="15"/>
+    </row>
+    <row r="26" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A26" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="K26" s="15"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="M27" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K28" s="15"/>
+    </row>
+    <row r="29" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A29" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="K29" s="15"/>
+    </row>
+    <row r="30" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="M30" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="14"/>
+    </row>
+    <row r="31" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="M31" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="14"/>
+    </row>
+    <row r="32" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="M32" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="14"/>
+    </row>
+    <row r="33" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="M33" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="15"/>
+      <c r="M34" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K35" s="15"/>
+    </row>
+    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="A36" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" s="15"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="15"/>
+      <c r="M37" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="9"/>
-      <c r="M18" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="M19" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="M20" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="M21" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-    </row>
-    <row r="22" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="M22" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-    </row>
-    <row r="23" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-    </row>
-    <row r="24" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-    </row>
-    <row r="25" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="M27" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+    </row>
+    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="A39" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" t="s">
+        <v>72</v>
+      </c>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="M40" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+    </row>
+    <row r="45" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="M16:O16"/>
+  <mergeCells count="12">
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="M34:O34"/>
     <mergeCell ref="M17:O17"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="M6:O6"/>
     <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Save terrain option added as well as f5 to load and f10 to save shortcuts in-game
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\Study\Project 1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A5FBB-EB04-4814-A454-AD73170E69A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C7E287-74AD-4DA4-AD31-395B494AA17D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="405" windowWidth="29040" windowHeight="15345" xr2:uid="{4499D1A8-1007-470A-BA2D-B0C0C3C062AE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
   <si>
     <t>Description</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>Make sure that the project structure is clear and flexible, focusing on the physics engine's structure</t>
+  </si>
+  <si>
+    <t>Working inputOutputModule</t>
+  </si>
+  <si>
+    <t>Have to option to save and load the game information (start location, terrain info, etc)</t>
   </si>
 </sst>
 </file>
@@ -377,7 +383,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -398,13 +404,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -723,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF05E52F-C67C-4F07-831F-FD1EB2BF79BD}">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,11 +779,11 @@
         <v>19</v>
       </c>
       <c r="L1" s="5"/>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
@@ -785,7 +792,7 @@
       <c r="Q2" s="5"/>
     </row>
     <row r="3" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>63</v>
       </c>
     </row>
@@ -798,11 +805,11 @@
       </c>
       <c r="C4" s="2"/>
       <c r="L4" s="14"/>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
     </row>
@@ -814,7 +821,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="20"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="12"/>
       <c r="L5" s="14"/>
       <c r="M5" s="15" t="s">
@@ -834,11 +841,11 @@
       <c r="E6" s="2"/>
       <c r="F6" s="12"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="16" t="s">
+      <c r="M6" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
     </row>
@@ -850,13 +857,13 @@
         <v>35</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="20"/>
+      <c r="F7" s="18"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="16" t="s">
+      <c r="M7" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
@@ -871,53 +878,43 @@
       <c r="E8" s="2"/>
       <c r="F8" s="12"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="16" t="s">
+      <c r="M8" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:17" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+    <row r="9" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="M9" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:17" s="15" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-    </row>
-    <row r="11" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="15" t="s">
-        <v>62</v>
       </c>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
     </row>
     <row r="12" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -926,264 +923,271 @@
       <c r="K12" s="1"/>
       <c r="L12" s="14"/>
       <c r="M12" s="15" t="s">
-        <v>39</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
     </row>
     <row r="13" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="M13" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="2"/>
       <c r="M14" s="13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
     </row>
     <row r="15" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>1</v>
       </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="M15" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
     </row>
     <row r="16" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="M16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+    </row>
+    <row r="17" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B17" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="15" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="9"/>
-      <c r="M17" s="16" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="9"/>
+      <c r="M18" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-    </row>
-    <row r="18" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+    </row>
+    <row r="19" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="M18" s="8" t="s">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="M19" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-    </row>
-    <row r="20" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="19" t="s">
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+    </row>
+    <row r="21" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="A21" s="17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="20"/>
-      <c r="M21" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="5"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>8</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="20"/>
-      <c r="M22" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="18"/>
+      <c r="M22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="M23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
+      <c r="E23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="M23" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="15"/>
-      <c r="M24" s="16" t="s">
+      <c r="D24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="M24" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="15"/>
+      <c r="M25" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K25" s="15"/>
-    </row>
-    <row r="26" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="19" t="s">
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K26" s="15"/>
+    </row>
+    <row r="27" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="A27" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="K26" s="15"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="K27" s="15"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>10</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="M27" s="16" t="s">
+      <c r="D28" s="15"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="M28" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K28" s="15"/>
-    </row>
-    <row r="29" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A29" s="19" t="s">
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K29" s="15"/>
+    </row>
+    <row r="30" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="K29" s="15"/>
-    </row>
-    <row r="30" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+      <c r="K30" s="15"/>
+    </row>
+    <row r="31" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="M30" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="14"/>
-    </row>
-    <row r="31" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>24</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="D31" s="2"/>
       <c r="M31" s="13" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="N31" s="13"/>
       <c r="O31" s="13"/>
       <c r="P31" s="14"/>
     </row>
-    <row r="32" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
       <c r="M32" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N32" s="13"/>
       <c r="O32" s="13"/>
       <c r="P32" s="14"/>
     </row>
-    <row r="33" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>36</v>
@@ -1191,96 +1195,112 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="M33" s="13" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="N33" s="13"/>
       <c r="O33" s="13"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="P33" s="14"/>
+    </row>
+    <row r="34" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="M34" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="N34" s="13"/>
+      <c r="O34" s="13"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>28</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>36</v>
       </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="15"/>
-      <c r="M34" s="16" t="s">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="15"/>
+      <c r="M35" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="N34" s="16"/>
-      <c r="O34" s="16"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K35" s="15"/>
-    </row>
-    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A36" s="19" t="s">
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K36" s="15"/>
+    </row>
+    <row r="37" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A37" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K36" s="15"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="K37" s="15"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>32</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>37</v>
       </c>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="15"/>
-      <c r="M37" s="16" t="s">
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="15"/>
+      <c r="M38" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="N37" s="16"/>
-      <c r="O37" s="16"/>
-    </row>
-    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A39" s="19" t="s">
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+    </row>
+    <row r="40" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A40" s="17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>71</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>72</v>
       </c>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="M40" s="15" t="s">
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="M41" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-    </row>
-    <row r="45" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="7"/>
+    <row r="45" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+    </row>
+    <row r="46" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="M18:O18"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M22:O22"/>
     <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M27:O27"/>
     <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="M17:O17"/>
     <mergeCell ref="M7:O7"/>
     <mergeCell ref="M8:O8"/>
   </mergeCells>

</xml_diff>